<commit_message>
Update .gitignore, add sample data files, and modify database connection script
</commit_message>
<xml_diff>
--- a/data/sample_data.xlsx
+++ b/data/sample_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e7eb7efc18aea852/Desktop/Projects/DataForge-AI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{E561112C-50A9-41E2-81C4-F5C6833C4E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD50C0DC-2913-4108-8849-B9D8A6663E01}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{E561112C-50A9-41E2-81C4-F5C6833C4E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{090C89E2-B35E-4DDF-9CD5-62122CB7158D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{022FA07E-FAD0-4912-866F-B3F0C853D20B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -60,31 +60,25 @@
     <t>Bob</t>
   </si>
   <si>
-    <t>Charli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David </t>
-  </si>
-  <si>
     <t>Eve</t>
   </si>
   <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>delhi</t>
-  </si>
-  <si>
-    <t>mumbai</t>
-  </si>
-  <si>
-    <t>haryana</t>
-  </si>
-  <si>
-    <t>pune</t>
-  </si>
-  <si>
-    <t>banglore</t>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Houston</t>
   </si>
 </sst>
 </file>
@@ -454,7 +448,7 @@
   <dimension ref="C3:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,10 +478,10 @@
         <v>5</v>
       </c>
       <c r="E4" s="1">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G4" s="1">
         <v>50000</v>
@@ -501,10 +495,10 @@
         <v>6</v>
       </c>
       <c r="E5" s="1">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G5" s="1">
         <v>60000</v>
@@ -515,16 +509,14 @@
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1">
-        <v>23</v>
-      </c>
-      <c r="F6" s="1">
-        <v>43</v>
+        <v>10</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G6" s="1">
-        <v>0</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.3">
@@ -532,14 +524,16 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="E7" s="1">
+        <v>35</v>
+      </c>
       <c r="F7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="1">
-        <v>5600</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.3">
@@ -547,34 +541,22 @@
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="1">
-        <v>54000</v>
+        <v>90000</v>
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C9" s="1">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="1">
-        <v>29</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="1">
-        <v>88000</v>
-      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>

</xml_diff>